<commit_message>
create database, add 'fluxo-formando' on rascunho, create conection.php.
</commit_message>
<xml_diff>
--- a/Rascunho/Rascunho Tabela.xlsx
+++ b/Rascunho/Rascunho Tabela.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t xml:space="preserve"> Tabela   cursos</t>
   </si>
@@ -137,6 +137,36 @@
   <si>
     <t>Tabela Meus cursos</t>
   </si>
+  <si>
+    <t>Tabela descricao</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>descicao-resumida</t>
+  </si>
+  <si>
+    <t>descicao-detalhada</t>
+  </si>
+  <si>
+    <t>perfil</t>
+  </si>
+  <si>
+    <t>idperfil</t>
+  </si>
+  <si>
+    <t>nomeperfil</t>
+  </si>
+  <si>
+    <t>categoria</t>
+  </si>
+  <si>
+    <t>idcategoria</t>
+  </si>
+  <si>
+    <t>nomecategoria</t>
+  </si>
 </sst>
 </file>
 
@@ -159,15 +189,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -190,14 +226,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F16"/>
+  <dimension ref="B3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -555,7 +607,7 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -570,7 +622,7 @@
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -630,19 +682,53 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
+    <row r="13" spans="2:6">
+      <c r="E13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
     <row r="14" spans="2:6">
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="1" t="s">
         <v>26</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create crud files for admin - IN PROCESS
</commit_message>
<xml_diff>
--- a/Rascunho/Rascunho Tabela.xlsx
+++ b/Rascunho/Rascunho Tabela.xlsx
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>